<commit_message>
Ho finito! Leggete please e ditemi se va tutto bene!
</commit_message>
<xml_diff>
--- a/Data/Analyzed/DataAnalyzed.xlsx
+++ b/Data/Analyzed/DataAnalyzed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="126">
   <si>
     <t>Costanti</t>
   </si>
@@ -239,12 +239,6 @@
     <t>measure</t>
   </si>
   <si>
-    <t>C final error</t>
-  </si>
-  <si>
-    <t>C error rel</t>
-  </si>
-  <si>
     <t>C vero</t>
   </si>
   <si>
@@ -385,15 +379,43 @@
   <si>
     <t>Dev. Std.</t>
   </si>
+  <si>
+    <t>Set</t>
+  </si>
+  <si>
+    <t>$c$</t>
+  </si>
+  <si>
+    <t>$\sigma_{sist}$</t>
+  </si>
+  <si>
+    <t>$\sigma_{sist}$ Rel.</t>
+  </si>
+  <si>
+    <t>$c_{rand}$</t>
+  </si>
+  <si>
+    <t>$\sigma_c$</t>
+  </si>
+  <si>
+    <t>$\sigma_c$ rel</t>
+  </si>
+  <si>
+    <t>$c$ \si{\meter\per\second}</t>
+  </si>
+  <si>
+    <t>Err. rel.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
-    <numFmt numFmtId="173" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -628,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -669,9 +691,10 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5079,10 +5102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23:L23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J28" sqref="H27:J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5111,6 +5134,34 @@
       <c r="D2" t="s">
         <v>27</v>
       </c>
+      <c r="H2" t="str">
+        <f>'Misura di c'!B62</f>
+        <v>C final</v>
+      </c>
+      <c r="I2" t="str">
+        <f>'Misura di c'!C62</f>
+        <v>C error strum</v>
+      </c>
+      <c r="J2" t="str">
+        <f>'Misura di c'!D62</f>
+        <v>error strum rel</v>
+      </c>
+      <c r="K2" t="str">
+        <f>'Misura di c'!E62</f>
+        <v>C error random</v>
+      </c>
+      <c r="L2" t="str">
+        <f>'Misura di c'!F62</f>
+        <v>error rand rel</v>
+      </c>
+      <c r="M2" t="str">
+        <f>'Misura di c'!G62</f>
+        <v>C error tot</v>
+      </c>
+      <c r="N2" t="str">
+        <f>'Misura di c'!H62</f>
+        <v>Error rel</v>
+      </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
@@ -5126,6 +5177,34 @@
         <f>C3/B3</f>
         <v>6.3291139240506328E-3</v>
       </c>
+      <c r="H3">
+        <f>'Misura di c'!B63</f>
+        <v>297591064.4613865</v>
+      </c>
+      <c r="I3">
+        <f>'Misura di c'!C63</f>
+        <v>1735641.7089090352</v>
+      </c>
+      <c r="J3">
+        <f>'Misura di c'!D63</f>
+        <v>5.8323045150915171E-3</v>
+      </c>
+      <c r="K3">
+        <f>'Misura di c'!E63</f>
+        <v>2156820.2864050595</v>
+      </c>
+      <c r="L3">
+        <f>'Misura di c'!F63</f>
+        <v>7.2475976061603647E-3</v>
+      </c>
+      <c r="M3">
+        <f>'Misura di c'!G63</f>
+        <v>2768451.8940290581</v>
+      </c>
+      <c r="N3" s="39">
+        <f>'Misura di c'!H63</f>
+        <v>9.3028730517823541E-3</v>
+      </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
@@ -5141,6 +5220,34 @@
         <f t="shared" ref="D4:D7" si="0">C4/B4</f>
         <v>3.0303030303030304E-2</v>
       </c>
+      <c r="H4">
+        <f>'Misura di c (2)'!A41</f>
+        <v>307778654.13901591</v>
+      </c>
+      <c r="I4">
+        <f>'Misura di c (2)'!B41</f>
+        <v>2539199.7606219756</v>
+      </c>
+      <c r="J4">
+        <f>'Misura di c (2)'!C41</f>
+        <v>8.2500840343368402E-3</v>
+      </c>
+      <c r="K4">
+        <f>'Misura di c (2)'!D41</f>
+        <v>4268475.1967464751</v>
+      </c>
+      <c r="L4">
+        <f>'Misura di c (2)'!E41</f>
+        <v>1.3868652485622059E-2</v>
+      </c>
+      <c r="M4">
+        <f>'Misura di c (2)'!F41</f>
+        <v>6807674.9573684502</v>
+      </c>
+      <c r="N4" s="39">
+        <f>'Misura di c (2)'!G41</f>
+        <v>2.2118736519958899E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
@@ -5156,6 +5263,34 @@
         <f t="shared" si="0"/>
         <v>6.1162079510703364E-3</v>
       </c>
+      <c r="H5">
+        <f>'Misura di c (3)'!B43</f>
+        <v>298030813.56154925</v>
+      </c>
+      <c r="I5">
+        <f>'Misura di c (3)'!C43</f>
+        <v>2456744.2684852304</v>
+      </c>
+      <c r="J5">
+        <f>'Misura di c (3)'!D43</f>
+        <v>8.2432559208441177E-3</v>
+      </c>
+      <c r="K5">
+        <f>'Misura di c (3)'!E43</f>
+        <v>1105556.1943434244</v>
+      </c>
+      <c r="L5">
+        <f>'Misura di c (3)'!F43</f>
+        <v>3.7095365446670673E-3</v>
+      </c>
+      <c r="M5">
+        <f>'Misura di c (3)'!G43</f>
+        <v>2694039.142177809</v>
+      </c>
+      <c r="N5" s="39">
+        <f>'Misura di c (3)'!H43</f>
+        <v>9.0394651143058287E-3</v>
+      </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
@@ -5211,20 +5346,64 @@
       <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
+      <c r="H10" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="H11" s="4"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="34"/>
+      <c r="H11" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="I11" s="31" t="str">
+        <f>"\num{" &amp; TEXT(H3/100000000,"0.00") &amp; "E+08}"</f>
+        <v>\num{2.98E+08}</v>
+      </c>
+      <c r="J11" s="31" t="str">
+        <f>"\num{" &amp; TEXT(I3/100000000,"0.00") &amp; "E+08}"</f>
+        <v>\num{0.02E+08}</v>
+      </c>
+      <c r="K11" s="34">
+        <f>J3</f>
+        <v>5.8323045150915171E-3</v>
+      </c>
+      <c r="L11" s="31" t="str">
+        <f>"\num{" &amp; TEXT(K3/100000000,"0.00") &amp; "E+08}"</f>
+        <v>\num{0.02E+08}</v>
+      </c>
+      <c r="M11" s="34">
+        <f>L3</f>
+        <v>7.2475976061603647E-3</v>
+      </c>
+      <c r="N11" s="31" t="str">
+        <f>"\num{" &amp; TEXT(M3/100000000,"0.00") &amp; "E+08}"</f>
+        <v>\num{0.03E+08}</v>
+      </c>
+      <c r="O11" s="34">
+        <f>N3</f>
+        <v>9.3028730517823541E-3</v>
+      </c>
+      <c r="P11" s="31"/>
       <c r="Q11" s="31"/>
     </row>
     <row r="12" spans="1:17">
@@ -5234,13 +5413,37 @@
       <c r="B12" s="1">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="32"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="32"/>
+      <c r="H12" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="I12" s="33" t="str">
+        <f t="shared" ref="I12:J12" si="1">"\num{" &amp; TEXT(H4/100000000,"0.00") &amp; "E+08}"</f>
+        <v>\num{3.08E+08}</v>
+      </c>
+      <c r="J12" s="32" t="str">
+        <f t="shared" si="1"/>
+        <v>\num{0.03E+08}</v>
+      </c>
+      <c r="K12" s="33">
+        <f t="shared" ref="K12:K13" si="2">J4</f>
+        <v>8.2500840343368402E-3</v>
+      </c>
+      <c r="L12" s="32" t="str">
+        <f t="shared" ref="L12:L13" si="3">"\num{" &amp; TEXT(K4/100000000,"0.00") &amp; "E+08}"</f>
+        <v>\num{0.04E+08}</v>
+      </c>
+      <c r="M12" s="33">
+        <f t="shared" ref="M12:M13" si="4">L4</f>
+        <v>1.3868652485622059E-2</v>
+      </c>
+      <c r="N12" s="32" t="str">
+        <f t="shared" ref="N12:N13" si="5">"\num{" &amp; TEXT(M4/100000000,"0.00") &amp; "E+08}"</f>
+        <v>\num{0.07E+08}</v>
+      </c>
+      <c r="O12" s="33">
+        <f t="shared" ref="O12:O13" si="6">N4</f>
+        <v>2.2118736519958899E-2</v>
+      </c>
       <c r="P12" s="33"/>
       <c r="Q12" s="32"/>
     </row>
@@ -5251,13 +5454,37 @@
       <c r="B13" s="1">
         <v>0.252</v>
       </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="34"/>
+      <c r="H13" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I13" s="31" t="str">
+        <f t="shared" ref="I13:J13" si="7">"\num{" &amp; TEXT(H5/100000000,"0.00") &amp; "E+08}"</f>
+        <v>\num{2.98E+08}</v>
+      </c>
+      <c r="J13" s="31" t="str">
+        <f t="shared" si="7"/>
+        <v>\num{0.02E+08}</v>
+      </c>
+      <c r="K13" s="34">
+        <f t="shared" si="2"/>
+        <v>8.2432559208441177E-3</v>
+      </c>
+      <c r="L13" s="31" t="str">
+        <f t="shared" si="3"/>
+        <v>\num{0.01E+08}</v>
+      </c>
+      <c r="M13" s="34">
+        <f t="shared" si="4"/>
+        <v>3.7095365446670673E-3</v>
+      </c>
+      <c r="N13" s="31" t="str">
+        <f t="shared" si="5"/>
+        <v>\num{0.03E+08}</v>
+      </c>
+      <c r="O13" s="34">
+        <f t="shared" si="6"/>
+        <v>9.0394651143058287E-3</v>
+      </c>
       <c r="P13" s="34"/>
       <c r="Q13" s="31"/>
     </row>
@@ -5266,6 +5493,7 @@
       <c r="J14" s="32"/>
       <c r="K14" s="33"/>
       <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
       <c r="N14" s="32"/>
       <c r="O14" s="32"/>
       <c r="P14" s="33"/>
@@ -5321,7 +5549,7 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B18">
         <f>299792458/1.000276</f>
@@ -5417,11 +5645,11 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <f t="shared" ref="E22:F22" si="1">(E$21-$C22)/SQRT(E$20^2+$B22^2)</f>
+        <f t="shared" ref="E22:F22" si="8">(E$21-$C22)/SQRT(E$20^2+$B22^2)</f>
         <v>1.3862428673794263</v>
       </c>
       <c r="F22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.11383843776742338</v>
       </c>
       <c r="I22" s="32"/>
@@ -5446,15 +5674,15 @@
         <v>307778654.13901591</v>
       </c>
       <c r="D23">
-        <f t="shared" ref="D23:F24" si="2">(D$21-$C23)/SQRT(D$20^2+$B23^2)</f>
+        <f t="shared" ref="D23:F24" si="9">(D$21-$C23)/SQRT(D$20^2+$B23^2)</f>
         <v>-1.3862428673794263</v>
       </c>
       <c r="E23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>-1.3314251771209229</v>
       </c>
       <c r="I23" s="31"/>
@@ -5479,15 +5707,15 @@
         <v>298030813.56154925</v>
       </c>
       <c r="D24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>-0.11383843776742338</v>
       </c>
       <c r="E24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1.3314251771209229</v>
       </c>
       <c r="F24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I24" s="32"/>
@@ -5548,14 +5776,14 @@
         <f>C27*A27</f>
         <v>3.8828080740541106E-5</v>
       </c>
-      <c r="H27" t="s">
-        <v>58</v>
-      </c>
-      <c r="I27" t="s">
-        <v>70</v>
-      </c>
-      <c r="J27" t="s">
-        <v>71</v>
+      <c r="H27" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="N27" s="31"/>
       <c r="O27" s="34"/>
@@ -5564,31 +5792,31 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28">
-        <f t="shared" ref="A28:A29" si="3">C23</f>
+        <f t="shared" ref="A28:A29" si="10">C23</f>
         <v>307778654.13901591</v>
       </c>
       <c r="B28">
-        <f t="shared" ref="B28" si="4">B23</f>
+        <f t="shared" ref="B28" si="11">B23</f>
         <v>6807674.9573684502</v>
       </c>
       <c r="C28">
-        <f t="shared" ref="C28:C29" si="5">B28^-2</f>
+        <f t="shared" ref="C28:C29" si="12">B28^-2</f>
         <v>2.1577562187362705E-14</v>
       </c>
       <c r="D28">
-        <f t="shared" ref="D28:D29" si="6">C28*A28</f>
+        <f t="shared" ref="D28:D29" si="13">C28*A28</f>
         <v>6.6411130496274134E-6</v>
       </c>
-      <c r="H28">
-        <f>D30/C30</f>
-        <v>298558558.72766507</v>
-      </c>
-      <c r="I28">
-        <f>C30^-0.5</f>
-        <v>1857484.7945189711</v>
-      </c>
-      <c r="J28">
-        <f>I28/H28</f>
+      <c r="H28" s="31" t="str">
+        <f>"\num{" &amp; TEXT(D30/(C30*100000000),"0.00") &amp; "E+08}"</f>
+        <v>\num{2.99E+08}</v>
+      </c>
+      <c r="I28" s="34" t="str">
+        <f>"\num{" &amp; TEXT(C30^-0.5/100000000,"0.00") &amp; "E+08}"</f>
+        <v>\num{0.02E+08}</v>
+      </c>
+      <c r="J28" s="34">
+        <f>((D30/C30)/C30^-0.5)^-1</f>
         <v>6.2215091151123399E-3</v>
       </c>
       <c r="N28" s="32"/>
@@ -5598,7 +5826,7 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>298030813.56154925</v>
       </c>
       <c r="B29">
@@ -5606,11 +5834,11 @@
         <v>2694039.142177809</v>
       </c>
       <c r="C29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>1.3778190885467998E-13</v>
       </c>
       <c r="D29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>4.1063254390023501E-5</v>
       </c>
       <c r="N29" s="31"/>
@@ -5632,13 +5860,56 @@
       </c>
     </row>
     <row r="31" spans="1:17">
-      <c r="H31">
+      <c r="H31" t="e">
         <f>ABS(H28-B18)/I28</f>
-        <v>0.61975171372214444</v>
-      </c>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="34" spans="8:13">
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+    </row>
+    <row r="35" spans="8:13">
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+    </row>
+    <row r="36" spans="8:13">
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+    </row>
+    <row r="37" spans="8:13">
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="L37" s="34"/>
+      <c r="M37" s="31"/>
+    </row>
+    <row r="38" spans="8:13">
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="M38" s="32"/>
+    </row>
+    <row r="39" spans="8:13">
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5646,8 +5917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR66"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V37" sqref="V37:X37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5787,7 +6058,7 @@
       <c r="C9" s="1"/>
       <c r="E9" s="1"/>
       <c r="S9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:43" ht="15.75" thickBot="1">
@@ -5939,7 +6210,7 @@
     </row>
     <row r="12" spans="1:43" ht="15.75" thickBot="1">
       <c r="B12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -5984,7 +6255,7 @@
         <v>36</v>
       </c>
       <c r="T12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="U12" s="12" t="s">
         <v>20</v>
@@ -9164,10 +9435,10 @@
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>
       <c r="AQ33" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AR33" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:44">
@@ -9225,13 +9496,13 @@
       <c r="S37" s="2"/>
       <c r="U37" s="4"/>
       <c r="V37" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="W37" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="X37" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="X37" s="4" t="s">
-        <v>117</v>
       </c>
       <c r="AK37" s="35"/>
     </row>
@@ -9251,7 +9522,7 @@
       <c r="R38" s="2"/>
       <c r="S38" s="2"/>
       <c r="U38" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="V38" s="31" t="str">
         <f>"\num{" &amp; TEXT(O37/1000000,"0.00") &amp; "E6}"</f>
@@ -9348,28 +9619,28 @@
         <v>4.7232075755814305E-6</v>
       </c>
       <c r="K42" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L42" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="M42" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="L42" s="4" t="s">
+      <c r="N42" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="M42" s="4" t="s">
+      <c r="O42" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="N42" s="4" t="s">
+      <c r="P42" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q42" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="R42" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="O42" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="P42" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q42" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="R42" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="S42" s="2"/>
       <c r="AK42" s="35"/>
@@ -9469,7 +9740,7 @@
         <v>\num{8.13E+06}</v>
       </c>
       <c r="R44" s="33">
-        <f t="shared" ref="P44:R61" si="39">R14</f>
+        <f t="shared" ref="R44:R61" si="39">R14</f>
         <v>3.9843524928798821E-2</v>
       </c>
       <c r="AK44" s="35"/>
@@ -10285,13 +10556,13 @@
         <v>59</v>
       </c>
       <c r="D62" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E62" t="s">
         <v>60</v>
       </c>
       <c r="F62" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G62" t="s">
         <v>62</v>
@@ -10352,8 +10623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10627,7 +10898,7 @@
         <v>36</v>
       </c>
       <c r="T12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="U12" s="5" t="s">
         <v>20</v>
@@ -11922,64 +12193,64 @@
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
       <c r="V26" t="s">
+        <v>76</v>
+      </c>
+      <c r="W26" t="s">
+        <v>77</v>
+      </c>
+      <c r="X26" t="s">
         <v>78</v>
       </c>
-      <c r="W26" t="s">
+      <c r="Y26" t="s">
         <v>79</v>
       </c>
-      <c r="X26" t="s">
+      <c r="Z26" t="s">
         <v>80</v>
       </c>
-      <c r="Y26" t="s">
+      <c r="AA26" t="s">
         <v>81</v>
       </c>
-      <c r="Z26" t="s">
+      <c r="AB26" t="s">
         <v>82</v>
       </c>
-      <c r="AA26" t="s">
+      <c r="AC26" t="s">
         <v>83</v>
       </c>
-      <c r="AB26" t="s">
+      <c r="AD26" t="s">
         <v>84</v>
       </c>
-      <c r="AC26" t="s">
+      <c r="AE26" t="s">
         <v>85</v>
       </c>
-      <c r="AD26" t="s">
+      <c r="AF26" t="s">
         <v>86</v>
       </c>
-      <c r="AE26" t="s">
+      <c r="AG26" t="s">
         <v>87</v>
       </c>
-      <c r="AF26" t="s">
+      <c r="AH26" t="s">
         <v>88</v>
       </c>
-      <c r="AG26" t="s">
+      <c r="AI26" t="s">
         <v>89</v>
       </c>
-      <c r="AH26" t="s">
+      <c r="AJ26" t="s">
         <v>90</v>
       </c>
-      <c r="AI26" t="s">
+      <c r="AK26" t="s">
         <v>91</v>
       </c>
-      <c r="AJ26" t="s">
+      <c r="AL26" t="s">
         <v>92</v>
       </c>
-      <c r="AK26" t="s">
+      <c r="AM26" t="s">
         <v>93</v>
       </c>
-      <c r="AL26" t="s">
+      <c r="AN26" t="s">
         <v>94</v>
       </c>
-      <c r="AM26" t="s">
-        <v>95</v>
-      </c>
-      <c r="AN26" t="s">
-        <v>96</v>
-      </c>
       <c r="AO26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:41">
@@ -12222,13 +12493,13 @@
         <v>48</v>
       </c>
       <c r="C40" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D40" t="s">
         <v>49</v>
       </c>
       <c r="E40" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F40" t="s">
         <v>52</v>
@@ -12269,28 +12540,28 @@
         <v>2.2118736519958899E-2</v>
       </c>
       <c r="K41" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L41" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="M41" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="L41" s="4" t="s">
+      <c r="N41" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="M41" s="4" t="s">
+      <c r="O41" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="N41" s="4" t="s">
+      <c r="P41" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q41" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="R41" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="O41" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="P41" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q41" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="R41" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="S41" s="2"/>
       <c r="T41" s="2"/>
@@ -12300,7 +12571,7 @@
         <v>1</v>
       </c>
       <c r="L42" s="31" t="str">
-        <f t="shared" ref="L42:M57" si="18">"\num{" &amp; B13 &amp; "}"</f>
+        <f t="shared" ref="L42:M51" si="18">"\num{" &amp; B13 &amp; "}"</f>
         <v>\num{118}</v>
       </c>
       <c r="M42" s="31" t="str">
@@ -12324,7 +12595,7 @@
         <v>\num{8.38E+06}</v>
       </c>
       <c r="R42" s="34">
-        <f>R13</f>
+        <f t="shared" ref="R42:R51" si="19">R13</f>
         <v>4.9402382105029022E-2</v>
       </c>
     </row>
@@ -12344,23 +12615,23 @@
         <v>\num{908}</v>
       </c>
       <c r="N43" s="32" t="str">
-        <f t="shared" ref="N43:O58" si="19">"\num{" &amp; TEXT(D14/0.001, "00.00") &amp; "}"</f>
+        <f t="shared" ref="N43:O51" si="20">"\num{" &amp; TEXT(D14/0.001, "00.00") &amp; "}"</f>
         <v>\num{09.88}</v>
       </c>
       <c r="O43" s="32" t="str">
+        <f t="shared" si="20"/>
+        <v>\num{09.65}</v>
+      </c>
+      <c r="P43" s="32" t="str">
+        <f t="shared" ref="P43:Q43" si="21">"\num{" &amp; TEXT(O14/1000000, "0.00") &amp; "E+06}"</f>
+        <v>\num{290.74E+06}</v>
+      </c>
+      <c r="Q43" s="32" t="str">
+        <f t="shared" si="21"/>
+        <v>\num{7.58E+06}</v>
+      </c>
+      <c r="R43" s="33">
         <f t="shared" si="19"/>
-        <v>\num{09.65}</v>
-      </c>
-      <c r="P43" s="32" t="str">
-        <f t="shared" ref="P43:Q43" si="20">"\num{" &amp; TEXT(O14/1000000, "0.00") &amp; "E+06}"</f>
-        <v>\num{290.74E+06}</v>
-      </c>
-      <c r="Q43" s="32" t="str">
-        <f t="shared" si="20"/>
-        <v>\num{7.58E+06}</v>
-      </c>
-      <c r="R43" s="33">
-        <f>R14</f>
         <v>5.3242988088032683E-2</v>
       </c>
     </row>
@@ -12381,23 +12652,23 @@
         <v>\num{915}</v>
       </c>
       <c r="N44" s="31" t="str">
+        <f t="shared" si="20"/>
+        <v>\num{09.86}</v>
+      </c>
+      <c r="O44" s="34" t="str">
+        <f t="shared" si="20"/>
+        <v>\num{09.65}</v>
+      </c>
+      <c r="P44" s="34" t="str">
+        <f t="shared" ref="P44:Q44" si="22">"\num{" &amp; TEXT(O15/1000000, "0.00") &amp; "E+06}"</f>
+        <v>\num{316.03E+06}</v>
+      </c>
+      <c r="Q44" s="34" t="str">
+        <f t="shared" si="22"/>
+        <v>\num{8.24E+06}</v>
+      </c>
+      <c r="R44" s="34">
         <f t="shared" si="19"/>
-        <v>\num{09.86}</v>
-      </c>
-      <c r="O44" s="34" t="str">
-        <f t="shared" si="19"/>
-        <v>\num{09.65}</v>
-      </c>
-      <c r="P44" s="34" t="str">
-        <f t="shared" ref="P44:Q44" si="21">"\num{" &amp; TEXT(O15/1000000, "0.00") &amp; "E+06}"</f>
-        <v>\num{316.03E+06}</v>
-      </c>
-      <c r="Q44" s="34" t="str">
-        <f t="shared" si="21"/>
-        <v>\num{8.24E+06}</v>
-      </c>
-      <c r="R44" s="34">
-        <f>R15</f>
         <v>5.0037294071765312E-2</v>
       </c>
     </row>
@@ -12414,23 +12685,23 @@
         <v>\num{908}</v>
       </c>
       <c r="N45" s="32" t="str">
+        <f t="shared" si="20"/>
+        <v>\num{09.88}</v>
+      </c>
+      <c r="O45" s="32" t="str">
+        <f t="shared" si="20"/>
+        <v>\num{09.65}</v>
+      </c>
+      <c r="P45" s="32" t="str">
+        <f t="shared" ref="P45:Q45" si="23">"\num{" &amp; TEXT(O16/1000000, "0.00") &amp; "E+06}"</f>
+        <v>\num{290.38E+06}</v>
+      </c>
+      <c r="Q45" s="32" t="str">
+        <f t="shared" si="23"/>
+        <v>\num{7.57E+06}</v>
+      </c>
+      <c r="R45" s="33">
         <f t="shared" si="19"/>
-        <v>\num{09.88}</v>
-      </c>
-      <c r="O45" s="32" t="str">
-        <f t="shared" si="19"/>
-        <v>\num{09.65}</v>
-      </c>
-      <c r="P45" s="32" t="str">
-        <f t="shared" ref="P45:Q45" si="22">"\num{" &amp; TEXT(O16/1000000, "0.00") &amp; "E+06}"</f>
-        <v>\num{290.38E+06}</v>
-      </c>
-      <c r="Q45" s="32" t="str">
-        <f t="shared" si="22"/>
-        <v>\num{7.57E+06}</v>
-      </c>
-      <c r="R45" s="33">
-        <f>R16</f>
         <v>5.329404508379719E-2</v>
       </c>
     </row>
@@ -12447,23 +12718,23 @@
         <v>\num{963}</v>
       </c>
       <c r="N46" s="31" t="str">
+        <f t="shared" si="20"/>
+        <v>\num{09.87}</v>
+      </c>
+      <c r="O46" s="34" t="str">
+        <f t="shared" si="20"/>
+        <v>\num{09.62}</v>
+      </c>
+      <c r="P46" s="34" t="str">
+        <f t="shared" ref="P46:Q46" si="24">"\num{" &amp; TEXT(O17/1000000, "0.00") &amp; "E+06}"</f>
+        <v>\num{291.74E+06}</v>
+      </c>
+      <c r="Q46" s="34" t="str">
+        <f t="shared" si="24"/>
+        <v>\num{7.60E+06}</v>
+      </c>
+      <c r="R46" s="34">
         <f t="shared" si="19"/>
-        <v>\num{09.87}</v>
-      </c>
-      <c r="O46" s="34" t="str">
-        <f t="shared" si="19"/>
-        <v>\num{09.62}</v>
-      </c>
-      <c r="P46" s="34" t="str">
-        <f t="shared" ref="P46:Q46" si="23">"\num{" &amp; TEXT(O17/1000000, "0.00") &amp; "E+06}"</f>
-        <v>\num{291.74E+06}</v>
-      </c>
-      <c r="Q46" s="34" t="str">
-        <f t="shared" si="23"/>
-        <v>\num{7.60E+06}</v>
-      </c>
-      <c r="R46" s="34">
-        <f>R17</f>
         <v>5.3104839042376006E-2</v>
       </c>
     </row>
@@ -12480,23 +12751,23 @@
         <v>\num{1400}</v>
       </c>
       <c r="N47" s="32" t="str">
+        <f t="shared" si="20"/>
+        <v>\num{09.88}</v>
+      </c>
+      <c r="O47" s="32" t="str">
+        <f t="shared" si="20"/>
+        <v>\num{09.53}</v>
+      </c>
+      <c r="P47" s="32" t="str">
+        <f t="shared" ref="P47:Q47" si="25">"\num{" &amp; TEXT(O18/1000000, "0.00") &amp; "E+06}"</f>
+        <v>\num{317.87E+06}</v>
+      </c>
+      <c r="Q47" s="32" t="str">
+        <f t="shared" si="25"/>
+        <v>\num{8.29E+06}</v>
+      </c>
+      <c r="R47" s="33">
         <f t="shared" si="19"/>
-        <v>\num{09.88}</v>
-      </c>
-      <c r="O47" s="32" t="str">
-        <f t="shared" si="19"/>
-        <v>\num{09.53}</v>
-      </c>
-      <c r="P47" s="32" t="str">
-        <f t="shared" ref="P47:Q47" si="24">"\num{" &amp; TEXT(O18/1000000, "0.00") &amp; "E+06}"</f>
-        <v>\num{317.87E+06}</v>
-      </c>
-      <c r="Q47" s="32" t="str">
-        <f t="shared" si="24"/>
-        <v>\num{8.29E+06}</v>
-      </c>
-      <c r="R47" s="33">
-        <f>R18</f>
         <v>4.9825865751132382E-2</v>
       </c>
     </row>
@@ -12513,23 +12784,23 @@
         <v>\num{1395}</v>
       </c>
       <c r="N48" s="31" t="str">
+        <f t="shared" si="20"/>
+        <v>\num{09.88}</v>
+      </c>
+      <c r="O48" s="34" t="str">
+        <f t="shared" si="20"/>
+        <v>\num{09.54}</v>
+      </c>
+      <c r="P48" s="34" t="str">
+        <f t="shared" ref="P48:Q48" si="26">"\num{" &amp; TEXT(O19/1000000, "0.00") &amp; "E+06}"</f>
+        <v>\num{317.07E+06}</v>
+      </c>
+      <c r="Q48" s="34" t="str">
+        <f t="shared" si="26"/>
+        <v>\num{8.26E+06}</v>
+      </c>
+      <c r="R48" s="34">
         <f t="shared" si="19"/>
-        <v>\num{09.88}</v>
-      </c>
-      <c r="O48" s="34" t="str">
-        <f t="shared" si="19"/>
-        <v>\num{09.54}</v>
-      </c>
-      <c r="P48" s="34" t="str">
-        <f t="shared" ref="P48:Q48" si="25">"\num{" &amp; TEXT(O19/1000000, "0.00") &amp; "E+06}"</f>
-        <v>\num{317.07E+06}</v>
-      </c>
-      <c r="Q48" s="34" t="str">
-        <f t="shared" si="25"/>
-        <v>\num{8.26E+06}</v>
-      </c>
-      <c r="R48" s="34">
-        <f>R19</f>
         <v>4.9917987885225466E-2</v>
       </c>
     </row>
@@ -12546,23 +12817,23 @@
         <v>\num{1385}</v>
       </c>
       <c r="N49" s="32" t="str">
+        <f t="shared" si="20"/>
+        <v>\num{09.89}</v>
+      </c>
+      <c r="O49" s="32" t="str">
+        <f t="shared" si="20"/>
+        <v>\num{09.54}</v>
+      </c>
+      <c r="P49" s="32" t="str">
+        <f t="shared" ref="P49:Q49" si="27">"\num{" &amp; TEXT(O20/1000000, "0.00") &amp; "E+06}"</f>
+        <v>\num{306.08E+06}</v>
+      </c>
+      <c r="Q49" s="32" t="str">
+        <f t="shared" si="27"/>
+        <v>\num{7.98E+06}</v>
+      </c>
+      <c r="R49" s="33">
         <f t="shared" si="19"/>
-        <v>\num{09.89}</v>
-      </c>
-      <c r="O49" s="32" t="str">
-        <f t="shared" si="19"/>
-        <v>\num{09.54}</v>
-      </c>
-      <c r="P49" s="32" t="str">
-        <f t="shared" ref="P49:Q49" si="26">"\num{" &amp; TEXT(O20/1000000, "0.00") &amp; "E+06}"</f>
-        <v>\num{306.08E+06}</v>
-      </c>
-      <c r="Q49" s="32" t="str">
-        <f t="shared" si="26"/>
-        <v>\num{7.98E+06}</v>
-      </c>
-      <c r="R49" s="33">
-        <f>R20</f>
         <v>5.1227117999630846E-2</v>
       </c>
     </row>
@@ -12579,23 +12850,23 @@
         <v>\num{1396}</v>
       </c>
       <c r="N50" s="31" t="str">
+        <f t="shared" si="20"/>
+        <v>\num{09.88}</v>
+      </c>
+      <c r="O50" s="34" t="str">
+        <f t="shared" si="20"/>
+        <v>\num{09.54}</v>
+      </c>
+      <c r="P50" s="34" t="str">
+        <f t="shared" ref="P50:Q50" si="28">"\num{" &amp; TEXT(O21/1000000, "0.00") &amp; "E+06}"</f>
+        <v>\num{326.23E+06}</v>
+      </c>
+      <c r="Q50" s="34" t="str">
+        <f t="shared" si="28"/>
+        <v>\num{8.50E+06}</v>
+      </c>
+      <c r="R50" s="34">
         <f t="shared" si="19"/>
-        <v>\num{09.88}</v>
-      </c>
-      <c r="O50" s="34" t="str">
-        <f t="shared" si="19"/>
-        <v>\num{09.54}</v>
-      </c>
-      <c r="P50" s="34" t="str">
-        <f t="shared" ref="P50:Q50" si="27">"\num{" &amp; TEXT(O21/1000000, "0.00") &amp; "E+06}"</f>
-        <v>\num{326.23E+06}</v>
-      </c>
-      <c r="Q50" s="34" t="str">
-        <f t="shared" si="27"/>
-        <v>\num{8.50E+06}</v>
-      </c>
-      <c r="R50" s="34">
-        <f>R21</f>
         <v>4.8901959038654942E-2</v>
       </c>
     </row>
@@ -12612,23 +12883,23 @@
         <v>\num{1385}</v>
       </c>
       <c r="N51" s="32" t="str">
+        <f t="shared" si="20"/>
+        <v>\num{09.89}</v>
+      </c>
+      <c r="O51" s="32" t="str">
+        <f t="shared" si="20"/>
+        <v>\num{09.54}</v>
+      </c>
+      <c r="P51" s="32" t="str">
+        <f t="shared" ref="P51:Q51" si="29">"\num{" &amp; TEXT(O22/1000000, "0.00") &amp; "E+06}"</f>
+        <v>\num{310.89E+06}</v>
+      </c>
+      <c r="Q51" s="32" t="str">
+        <f t="shared" si="29"/>
+        <v>\num{8.10E+06}</v>
+      </c>
+      <c r="R51" s="33">
         <f t="shared" si="19"/>
-        <v>\num{09.89}</v>
-      </c>
-      <c r="O51" s="32" t="str">
-        <f t="shared" si="19"/>
-        <v>\num{09.54}</v>
-      </c>
-      <c r="P51" s="32" t="str">
-        <f t="shared" ref="P51:Q51" si="28">"\num{" &amp; TEXT(O22/1000000, "0.00") &amp; "E+06}"</f>
-        <v>\num{310.89E+06}</v>
-      </c>
-      <c r="Q51" s="32" t="str">
-        <f t="shared" si="28"/>
-        <v>\num{8.10E+06}</v>
-      </c>
-      <c r="R51" s="33">
-        <f>R22</f>
         <v>5.0640630467443978E-2</v>
       </c>
     </row>
@@ -12646,8 +12917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12683,7 +12954,7 @@
         <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:34">
@@ -12921,7 +13192,7 @@
         <v>36</v>
       </c>
       <c r="T12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="U12" s="38" t="s">
         <v>20</v>
@@ -14193,7 +14464,7 @@
         <v>61</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="S25" s="2"/>
     </row>
@@ -14469,28 +14740,28 @@
     </row>
     <row r="41" spans="2:21">
       <c r="K41" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L41" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="M41" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="L41" s="4" t="s">
+      <c r="N41" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="M41" s="4" t="s">
+      <c r="O41" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="N41" s="4" t="s">
+      <c r="P41" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q41" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="R41" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="O41" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="P41" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q41" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="R41" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="S41" s="2"/>
     </row>
@@ -14502,13 +14773,13 @@
         <v>48</v>
       </c>
       <c r="D42" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E42" t="s">
         <v>49</v>
       </c>
       <c r="F42" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G42" t="s">
         <v>52</v>
@@ -14544,7 +14815,7 @@
         <v>\num{7.74E+06}</v>
       </c>
       <c r="R42" s="34">
-        <f>R13</f>
+        <f t="shared" ref="R42:R51" si="21">R13</f>
         <v>2.8601034957064574E-2</v>
       </c>
       <c r="S42" s="2"/>
@@ -14592,23 +14863,23 @@
         <v>\num{1382}</v>
       </c>
       <c r="N43" s="32" t="str">
-        <f t="shared" ref="N43:O51" si="21">"\num{" &amp; TEXT(D14/0.001, "00.00") &amp; "}"</f>
+        <f t="shared" ref="N43:O51" si="22">"\num{" &amp; TEXT(D14/0.001, "00.00") &amp; "}"</f>
         <v>\num{10.31}</v>
       </c>
       <c r="O43" s="32" t="str">
+        <f t="shared" si="22"/>
+        <v>\num{09.54}</v>
+      </c>
+      <c r="P43" s="32" t="str">
+        <f t="shared" ref="P43:Q51" si="23">"\num{" &amp; TEXT(O14/1000000, "0.00") &amp; "E+06}"</f>
+        <v>\num{302.97E+06}</v>
+      </c>
+      <c r="Q43" s="32" t="str">
+        <f t="shared" si="23"/>
+        <v>\num{7.90E+06}</v>
+      </c>
+      <c r="R43" s="33">
         <f t="shared" si="21"/>
-        <v>\num{09.54}</v>
-      </c>
-      <c r="P43" s="32" t="str">
-        <f t="shared" ref="P43:Q51" si="22">"\num{" &amp; TEXT(O14/1000000, "0.00") &amp; "E+06}"</f>
-        <v>\num{302.97E+06}</v>
-      </c>
-      <c r="Q43" s="32" t="str">
-        <f t="shared" si="22"/>
-        <v>\num{7.90E+06}</v>
-      </c>
-      <c r="R43" s="33">
-        <f>R14</f>
         <v>2.8505803970906053E-2</v>
       </c>
     </row>
@@ -14625,23 +14896,23 @@
         <v>\num{1373}</v>
       </c>
       <c r="N44" s="31" t="str">
+        <f t="shared" si="22"/>
+        <v>\num{10.32}</v>
+      </c>
+      <c r="O44" s="34" t="str">
+        <f t="shared" si="22"/>
+        <v>\num{09.53}</v>
+      </c>
+      <c r="P44" s="34" t="str">
+        <f t="shared" si="23"/>
+        <v>\num{293.24E+06}</v>
+      </c>
+      <c r="Q44" s="34" t="str">
+        <f t="shared" si="23"/>
+        <v>\num{7.64E+06}</v>
+      </c>
+      <c r="R44" s="34">
         <f t="shared" si="21"/>
-        <v>\num{10.32}</v>
-      </c>
-      <c r="O44" s="34" t="str">
-        <f t="shared" si="21"/>
-        <v>\num{09.53}</v>
-      </c>
-      <c r="P44" s="34" t="str">
-        <f t="shared" si="22"/>
-        <v>\num{293.24E+06}</v>
-      </c>
-      <c r="Q44" s="34" t="str">
-        <f t="shared" si="22"/>
-        <v>\num{7.64E+06}</v>
-      </c>
-      <c r="R44" s="34">
-        <f>R15</f>
         <v>2.8663088852797947E-2</v>
       </c>
     </row>
@@ -14661,23 +14932,23 @@
         <v>\num{1395}</v>
       </c>
       <c r="N45" s="32" t="str">
+        <f t="shared" si="22"/>
+        <v>\num{10.33}</v>
+      </c>
+      <c r="O45" s="32" t="str">
+        <f t="shared" si="22"/>
+        <v>\num{09.53}</v>
+      </c>
+      <c r="P45" s="32" t="str">
+        <f t="shared" si="23"/>
+        <v>\num{293.46E+06}</v>
+      </c>
+      <c r="Q45" s="32" t="str">
+        <f t="shared" si="23"/>
+        <v>\num{7.65E+06}</v>
+      </c>
+      <c r="R45" s="33">
         <f t="shared" si="21"/>
-        <v>\num{10.33}</v>
-      </c>
-      <c r="O45" s="32" t="str">
-        <f t="shared" si="21"/>
-        <v>\num{09.53}</v>
-      </c>
-      <c r="P45" s="32" t="str">
-        <f t="shared" si="22"/>
-        <v>\num{293.46E+06}</v>
-      </c>
-      <c r="Q45" s="32" t="str">
-        <f t="shared" si="22"/>
-        <v>\num{7.65E+06}</v>
-      </c>
-      <c r="R45" s="33">
-        <f>R16</f>
         <v>2.8659231711239776E-2</v>
       </c>
     </row>
@@ -14698,23 +14969,23 @@
         <v>\num{1397}</v>
       </c>
       <c r="N46" s="31" t="str">
+        <f t="shared" si="22"/>
+        <v>\num{10.32}</v>
+      </c>
+      <c r="O46" s="34" t="str">
+        <f t="shared" si="22"/>
+        <v>\num{09.53}</v>
+      </c>
+      <c r="P46" s="34" t="str">
+        <f t="shared" si="23"/>
+        <v>\num{298.72E+06}</v>
+      </c>
+      <c r="Q46" s="34" t="str">
+        <f t="shared" si="23"/>
+        <v>\num{7.79E+06}</v>
+      </c>
+      <c r="R46" s="34">
         <f t="shared" si="21"/>
-        <v>\num{10.32}</v>
-      </c>
-      <c r="O46" s="34" t="str">
-        <f t="shared" si="21"/>
-        <v>\num{09.53}</v>
-      </c>
-      <c r="P46" s="34" t="str">
-        <f t="shared" si="22"/>
-        <v>\num{298.72E+06}</v>
-      </c>
-      <c r="Q46" s="34" t="str">
-        <f t="shared" si="22"/>
-        <v>\num{7.79E+06}</v>
-      </c>
-      <c r="R46" s="34">
-        <f>R17</f>
         <v>2.8572795164306764E-2</v>
       </c>
     </row>
@@ -14731,23 +15002,23 @@
         <v>\num{1396}</v>
       </c>
       <c r="N47" s="32" t="str">
+        <f t="shared" si="22"/>
+        <v>\num{10.32}</v>
+      </c>
+      <c r="O47" s="32" t="str">
+        <f t="shared" si="22"/>
+        <v>\num{09.52}</v>
+      </c>
+      <c r="P47" s="32" t="str">
+        <f t="shared" si="23"/>
+        <v>\num{296.03E+06}</v>
+      </c>
+      <c r="Q47" s="32" t="str">
+        <f t="shared" si="23"/>
+        <v>\num{7.72E+06}</v>
+      </c>
+      <c r="R47" s="33">
         <f t="shared" si="21"/>
-        <v>\num{10.32}</v>
-      </c>
-      <c r="O47" s="32" t="str">
-        <f t="shared" si="21"/>
-        <v>\num{09.52}</v>
-      </c>
-      <c r="P47" s="32" t="str">
-        <f t="shared" si="22"/>
-        <v>\num{296.03E+06}</v>
-      </c>
-      <c r="Q47" s="32" t="str">
-        <f t="shared" si="22"/>
-        <v>\num{7.72E+06}</v>
-      </c>
-      <c r="R47" s="33">
-        <f>R18</f>
         <v>2.8616377318931938E-2</v>
       </c>
     </row>
@@ -14764,23 +15035,23 @@
         <v>\num{1394}</v>
       </c>
       <c r="N48" s="31" t="str">
+        <f t="shared" si="22"/>
+        <v>\num{10.32}</v>
+      </c>
+      <c r="O48" s="34" t="str">
+        <f t="shared" si="22"/>
+        <v>\num{09.53}</v>
+      </c>
+      <c r="P48" s="34" t="str">
+        <f t="shared" si="23"/>
+        <v>\num{301.91E+06}</v>
+      </c>
+      <c r="Q48" s="34" t="str">
+        <f t="shared" si="23"/>
+        <v>\num{7.87E+06}</v>
+      </c>
+      <c r="R48" s="34">
         <f t="shared" si="21"/>
-        <v>\num{10.32}</v>
-      </c>
-      <c r="O48" s="34" t="str">
-        <f t="shared" si="21"/>
-        <v>\num{09.53}</v>
-      </c>
-      <c r="P48" s="34" t="str">
-        <f t="shared" si="22"/>
-        <v>\num{301.91E+06}</v>
-      </c>
-      <c r="Q48" s="34" t="str">
-        <f t="shared" si="22"/>
-        <v>\num{7.87E+06}</v>
-      </c>
-      <c r="R48" s="34">
-        <f>R19</f>
         <v>2.8522363110912493E-2</v>
       </c>
     </row>
@@ -14797,23 +15068,23 @@
         <v>\num{1399}</v>
       </c>
       <c r="N49" s="32" t="str">
+        <f t="shared" si="22"/>
+        <v>\num{10.34}</v>
+      </c>
+      <c r="O49" s="32" t="str">
+        <f t="shared" si="22"/>
+        <v>\num{09.54}</v>
+      </c>
+      <c r="P49" s="32" t="str">
+        <f t="shared" si="23"/>
+        <v>\num{299.49E+06}</v>
+      </c>
+      <c r="Q49" s="32" t="str">
+        <f t="shared" si="23"/>
+        <v>\num{7.81E+06}</v>
+      </c>
+      <c r="R49" s="33">
         <f t="shared" si="21"/>
-        <v>\num{10.34}</v>
-      </c>
-      <c r="O49" s="32" t="str">
-        <f t="shared" si="21"/>
-        <v>\num{09.54}</v>
-      </c>
-      <c r="P49" s="32" t="str">
-        <f t="shared" si="22"/>
-        <v>\num{299.49E+06}</v>
-      </c>
-      <c r="Q49" s="32" t="str">
-        <f t="shared" si="22"/>
-        <v>\num{7.81E+06}</v>
-      </c>
-      <c r="R49" s="33">
-        <f>R20</f>
         <v>2.8560487205637398E-2</v>
       </c>
     </row>
@@ -14830,23 +15101,23 @@
         <v>\num{1398}</v>
       </c>
       <c r="N50" s="31" t="str">
+        <f t="shared" si="22"/>
+        <v>\num{10.35}</v>
+      </c>
+      <c r="O50" s="34" t="str">
+        <f t="shared" si="22"/>
+        <v>\num{09.55}</v>
+      </c>
+      <c r="P50" s="34" t="str">
+        <f t="shared" si="23"/>
+        <v>\num{296.25E+06}</v>
+      </c>
+      <c r="Q50" s="34" t="str">
+        <f t="shared" si="23"/>
+        <v>\num{7.72E+06}</v>
+      </c>
+      <c r="R50" s="34">
         <f t="shared" si="21"/>
-        <v>\num{10.35}</v>
-      </c>
-      <c r="O50" s="34" t="str">
-        <f t="shared" si="21"/>
-        <v>\num{09.55}</v>
-      </c>
-      <c r="P50" s="34" t="str">
-        <f t="shared" si="22"/>
-        <v>\num{296.25E+06}</v>
-      </c>
-      <c r="Q50" s="34" t="str">
-        <f t="shared" si="22"/>
-        <v>\num{7.72E+06}</v>
-      </c>
-      <c r="R50" s="34">
-        <f>R21</f>
         <v>2.8612914424407724E-2</v>
       </c>
     </row>
@@ -14863,23 +15134,23 @@
         <v>\num{1395}</v>
       </c>
       <c r="N51" s="32" t="str">
+        <f t="shared" si="22"/>
+        <v>\num{10.32}</v>
+      </c>
+      <c r="O51" s="32" t="str">
+        <f t="shared" si="22"/>
+        <v>\num{09.53}</v>
+      </c>
+      <c r="P51" s="32" t="str">
+        <f t="shared" si="23"/>
+        <v>\num{302.01E+06}</v>
+      </c>
+      <c r="Q51" s="32" t="str">
+        <f t="shared" si="23"/>
+        <v>\num{7.87E+06}</v>
+      </c>
+      <c r="R51" s="33">
         <f t="shared" si="21"/>
-        <v>\num{10.32}</v>
-      </c>
-      <c r="O51" s="32" t="str">
-        <f t="shared" si="21"/>
-        <v>\num{09.53}</v>
-      </c>
-      <c r="P51" s="32" t="str">
-        <f t="shared" si="22"/>
-        <v>\num{302.01E+06}</v>
-      </c>
-      <c r="Q51" s="32" t="str">
-        <f t="shared" si="22"/>
-        <v>\num{7.87E+06}</v>
-      </c>
-      <c r="R51" s="33">
-        <f>R22</f>
         <v>2.8520693214440403E-2</v>
       </c>
     </row>

</xml_diff>